<commit_message>
Release draft demo version 0.3.1
</commit_message>
<xml_diff>
--- a/documents/radioserver_20150211trans.xlsx
+++ b/documents/radioserver_20150211trans.xlsx
@@ -207,19 +207,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9664,15 +9664,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>107949</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>317500</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9681,8 +9681,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="571500" y="3143249"/>
-          <a:ext cx="4352925" cy="1771651"/>
+          <a:off x="342900" y="3282949"/>
+          <a:ext cx="4686300" cy="1835151"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9715,8 +9715,9 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="12000" b="1">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="11000" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -9726,7 +9727,7 @@
             <a:t>サ</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="12000" b="1">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="11000" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -9736,7 +9737,7 @@
             <a:t>-</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="12000" b="1">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="11000" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -9746,7 +9747,7 @@
             <a:t>バ</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="12000" b="1">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="11000" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -9755,7 +9756,7 @@
             </a:rPr>
             <a:t>-</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="12000" b="1">
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="11000" b="1">
             <a:solidFill>
               <a:schemeClr val="bg1"/>
             </a:solidFill>
@@ -9769,16 +9770,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>69474</xdr:rowOff>
+      <xdr:rowOff>145674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9787,8 +9788,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="542925" y="1910974"/>
-          <a:ext cx="4321175" cy="2191126"/>
+          <a:off x="746125" y="1720474"/>
+          <a:ext cx="4321175" cy="1810126"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14219,8 +14220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:BJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D2" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14233,88 +14234,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:62" ht="13.5" customHeight="1">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="P2" s="9" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="P2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="V2" s="6" t="s">
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="V2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="AB2" s="6" t="s">
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="AB2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AH2" s="6" t="s">
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AH2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AN2" s="6" t="s">
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AN2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="6"/>
-      <c r="AT2" s="6" t="s">
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AT2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AU2" s="6"/>
-      <c r="AV2" s="6"/>
-      <c r="AZ2" s="6" t="s">
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AZ2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="BA2" s="6"/>
-      <c r="BB2" s="6"/>
-      <c r="BG2" s="6" t="s">
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BG2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="BH2" s="6"/>
-      <c r="BI2" s="6"/>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5"/>
     </row>
     <row r="3" spans="3:62" ht="13.5" customHeight="1">
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="6"/>
-      <c r="AT3" s="6"/>
-      <c r="AU3" s="6"/>
-      <c r="AV3" s="6"/>
-      <c r="AZ3" s="6"/>
-      <c r="BA3" s="6"/>
-      <c r="BB3" s="6"/>
-      <c r="BG3" s="6"/>
-      <c r="BH3" s="6"/>
-      <c r="BI3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AT3" s="5"/>
+      <c r="AU3" s="5"/>
+      <c r="AV3" s="5"/>
+      <c r="AZ3" s="5"/>
+      <c r="BA3" s="5"/>
+      <c r="BB3" s="5"/>
+      <c r="BG3" s="5"/>
+      <c r="BH3" s="5"/>
+      <c r="BI3" s="5"/>
     </row>
     <row r="5" spans="3:62">
       <c r="I5" s="2"/>
@@ -14322,11 +14323,11 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -14369,11 +14370,11 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -14416,11 +14417,11 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -14463,11 +14464,11 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
@@ -14510,11 +14511,11 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -14557,11 +14558,11 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
@@ -14604,11 +14605,11 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -14651,11 +14652,11 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
@@ -14698,11 +14699,11 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -14745,11 +14746,11 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
@@ -14792,11 +14793,11 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -14839,11 +14840,11 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
@@ -14886,11 +14887,11 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -14933,11 +14934,11 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
@@ -14980,11 +14981,11 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
@@ -15027,11 +15028,11 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
@@ -15074,11 +15075,11 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -15121,11 +15122,11 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
@@ -15168,11 +15169,11 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
@@ -15215,11 +15216,11 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
@@ -15262,11 +15263,11 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
@@ -15309,11 +15310,11 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
@@ -15356,11 +15357,11 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
@@ -15403,11 +15404,11 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
@@ -15450,11 +15451,11 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
@@ -15497,11 +15498,11 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
@@ -15548,42 +15549,42 @@
       <c r="S32" s="3"/>
     </row>
     <row r="34" spans="9:13">
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
     </row>
     <row r="35" spans="9:13">
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
     </row>
     <row r="36" spans="9:13">
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="I34:M36"/>
+    <mergeCell ref="AZ2:BB3"/>
+    <mergeCell ref="AT2:AV3"/>
+    <mergeCell ref="O5:S30"/>
+    <mergeCell ref="AN2:AP3"/>
+    <mergeCell ref="AH2:AJ3"/>
     <mergeCell ref="BG2:BI3"/>
     <mergeCell ref="C2:E3"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="P2:R3"/>
     <mergeCell ref="V2:X3"/>
     <mergeCell ref="AB2:AD3"/>
-    <mergeCell ref="I34:M36"/>
-    <mergeCell ref="AZ2:BB3"/>
-    <mergeCell ref="AT2:AV3"/>
-    <mergeCell ref="O5:S30"/>
-    <mergeCell ref="AN2:AP3"/>
-    <mergeCell ref="AH2:AJ3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>